<commit_message>
[dev] Complete Impl for task
</commit_message>
<xml_diff>
--- a/PoppuloTask/poppulo_techtask.xlsx
+++ b/PoppuloTask/poppulo_techtask.xlsx
@@ -1,28 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25401"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{44BC33F6-1F78-47A8-A3E5-A7983FFCB0E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Projects\Personal\HiringTask_Poppulo\PoppuloTask\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F295A8-B6E5-45B2-BCB1-FAB32498188C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="poppulo_techtask" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -528,7 +521,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -881,11 +874,13 @@
   </sheetPr>
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -902,7 +897,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -919,7 +914,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -936,7 +931,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -953,7 +948,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
@@ -970,7 +965,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
@@ -987,7 +982,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>29</v>
       </c>
@@ -1004,7 +999,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>32</v>
       </c>
@@ -1021,7 +1016,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>35</v>
       </c>
@@ -1038,7 +1033,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>38</v>
       </c>
@@ -1055,7 +1050,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>41</v>
       </c>
@@ -1072,7 +1067,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>44</v>
       </c>
@@ -1089,7 +1084,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>47</v>
       </c>
@@ -1106,7 +1101,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>50</v>
       </c>
@@ -1123,7 +1118,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>53</v>
       </c>
@@ -1140,7 +1135,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>56</v>
       </c>
@@ -1157,7 +1152,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>59</v>
       </c>
@@ -1174,7 +1169,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>62</v>
       </c>
@@ -1191,7 +1186,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>65</v>
       </c>
@@ -1208,7 +1203,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>68</v>
       </c>
@@ -1225,7 +1220,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>71</v>
       </c>
@@ -1242,7 +1237,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>74</v>
       </c>
@@ -1259,7 +1254,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>77</v>
       </c>
@@ -1276,7 +1271,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>80</v>
       </c>
@@ -1293,7 +1288,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>83</v>
       </c>
@@ -1310,7 +1305,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>86</v>
       </c>
@@ -1327,7 +1322,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>89</v>
       </c>
@@ -1344,7 +1339,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>92</v>
       </c>
@@ -1361,7 +1356,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>95</v>
       </c>
@@ -1378,7 +1373,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>98</v>
       </c>
@@ -1395,7 +1390,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>101</v>
       </c>
@@ -1412,7 +1407,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>104</v>
       </c>
@@ -1429,7 +1424,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>107</v>
       </c>
@@ -1446,7 +1441,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>110</v>
       </c>
@@ -1463,7 +1458,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>113</v>
       </c>
@@ -1480,7 +1475,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>116</v>
       </c>
@@ -1497,7 +1492,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>119</v>
       </c>
@@ -1514,7 +1509,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>122</v>
       </c>
@@ -1531,7 +1526,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>125</v>
       </c>
@@ -1548,7 +1543,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>128</v>
       </c>
@@ -1565,7 +1560,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>131</v>
       </c>
@@ -1582,7 +1577,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>135</v>
       </c>
@@ -1599,7 +1594,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>138</v>
       </c>
@@ -1616,7 +1611,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>141</v>
       </c>
@@ -1633,7 +1628,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>144</v>
       </c>
@@ -1650,7 +1645,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>147</v>
       </c>
@@ -1667,7 +1662,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>150</v>
       </c>
@@ -1684,7 +1679,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>153</v>
       </c>
@@ -1701,7 +1696,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>156</v>
       </c>
@@ -1718,7 +1713,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>159</v>
       </c>
@@ -1735,7 +1730,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>162</v>
       </c>

</xml_diff>